<commit_message>
tests des effectifs de transition en cours
</commit_message>
<xml_diff>
--- a/TRANSITIONS.xlsx
+++ b/TRANSITIONS.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/ef77bd1ebbbb3aed/modele_emprunteur/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="5" documentId="11_71B21E0D5A8F15B1752002EE9ABD93438013B7EE" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B91323E1-ADE4-4EDA-9FDB-002AFA6D3D32}"/>
+  <xr:revisionPtr revIDLastSave="12" documentId="11_71B21E0D5A8F15B1752002EE9ABD93438013B7EE" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{560123DC-2F7E-4DE8-917F-73E621B75405}"/>
   <bookViews>
-    <workbookView xWindow="19935" yWindow="1080" windowWidth="17175" windowHeight="15435" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="12075" yWindow="-21225" windowWidth="20310" windowHeight="16980" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -235,7 +235,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="4">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -276,11 +276,22 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="hair">
+        <color indexed="64"/>
+      </left>
+      <right style="hair">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -300,6 +311,9 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -644,10 +658,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B2:I11"/>
+  <dimension ref="B2:I12"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="C1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A2" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -851,6 +865,14 @@
         <v>36</v>
       </c>
     </row>
+    <row r="12" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="D12" s="8"/>
+      <c r="E12" s="8"/>
+      <c r="F12" s="8"/>
+      <c r="G12" s="8"/>
+      <c r="H12" s="8"/>
+      <c r="I12" s="8"/>
+    </row>
   </sheetData>
   <mergeCells count="2">
     <mergeCell ref="B6:B11"/>

</xml_diff>